<commit_message>
Actividad clase 8 excel
</commit_message>
<xml_diff>
--- a/Primera Entrega/Clase 8- Memoria/Alumnos/David Tellez/Actividad 8  Excel.xlsx
+++ b/Primera Entrega/Clase 8- Memoria/Alumnos/David Tellez/Actividad 8  Excel.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Tellez\Desktop\Actividad 6\Mochila_0522TDIIFN2C4LAED0522PT-\Primera Entrega\Clase 8- Memoria\Alumnos\David Tellez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04751C85-876E-48DB-9466-4077D348B09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A1561C5-860D-4D12-92AD-66637BEE1902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13470" yWindow="1860" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{62307458-C259-40A6-A30A-48E43D1C5DF6}"/>
+    <workbookView xWindow="0" yWindow="1860" windowWidth="28800" windowHeight="11385" xr2:uid="{62307458-C259-40A6-A30A-48E43D1C5DF6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table005 (Page 5)" sheetId="3" r:id="rId1"/>
-    <sheet name="Table004 (Page 4)" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja1" sheetId="1" r:id="rId3"/>
+    <sheet name="Table004 (Page 4)" sheetId="2" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="1" hidden="1">'Table004 (Page 4)'!$A$1:$B$16</definedName>
-    <definedName name="DatosExternos_2" localSheetId="0" hidden="1">'Table005 (Page 5)'!$A$1:$B$1</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'Table004 (Page 4)'!$A$1:$B$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Column1</t>
   </si>
@@ -145,12 +144,6 @@
   </si>
   <si>
     <t>78,2 MB</t>
-  </si>
-  <si>
-    <t>Columna1</t>
-  </si>
-  <si>
-    <t>Columna2</t>
   </si>
   <si>
     <t>Column3</t>
@@ -205,13 +198,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -238,17 +225,6 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_2" connectionId="2" xr16:uid="{9684BE41-3492-44EA-AE45-F62D60C74A42}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="3">
-    <queryTableFields count="2">
-      <queryTableField id="1" name="Column1" tableColumnId="1"/>
-      <queryTableField id="2" name="Column2" tableColumnId="2"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{E5403D67-EB7D-4264-BA8A-313332A1148F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="5" unboundColumnsRight="2">
     <queryTableFields count="4">
@@ -262,25 +238,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE0DFB54-6991-44E7-9D8D-24EF9F9DE426}" name="Table005__Page_5" displayName="Table005__Page_5" ref="A1:B11" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B11" xr:uid="{FE0DFB54-6991-44E7-9D8D-24EF9F9DE426}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7BB30BB2-B246-4338-8A62-7FF392942D8D}" uniqueName="1" name="Columna1" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{01DAB91F-1E50-401D-BDD0-157BF734308D}" uniqueName="2" name="Columna2" queryTableFieldId="2" dataDxfId="2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F2E3DEB-3EB0-4F82-81CE-9A0402BB27A0}" name="Table004__Page_4" displayName="Table004__Page_4" ref="A1:D16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D16" xr:uid="{6F2E3DEB-3EB0-4F82-81CE-9A0402BB27A0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D16">
     <sortCondition ref="D1:D16"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1B32B5F1-065A-4D0E-9DD7-8BC01DE93699}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{2F5F3B6D-4F29-4984-A2AD-52F0DC451E28}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{1B32B5F1-065A-4D0E-9DD7-8BC01DE93699}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{2F5F3B6D-4F29-4984-A2AD-52F0DC451E28}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{3C597405-A346-4239-8999-F27C30ED7E88}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{18FB6E61-9743-4023-B6BB-90A2B2E00D4C}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
@@ -584,36 +549,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DED637-923A-44F2-9841-F7332EC4F8D7}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6611437-6AC3-4B0B-BB09-A67C94D88807}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -635,10 +570,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -854,7 +789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74434F10-7C64-4A5C-BC63-70BB3A24F192}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>